<commit_message>
feat: crawl data by date
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,166 +397,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>3 tháng</v>
-      </c>
-      <c r="C1" t="str">
-        <v>6 tháng</v>
-      </c>
-      <c r="D1" t="str">
-        <v>9 tháng</v>
-      </c>
-      <c r="E1" t="str">
-        <v>1 năm</v>
-      </c>
-      <c r="F1" t="str">
-        <v>2 năm</v>
-      </c>
-      <c r="G1" t="str">
-        <v>3 năm</v>
-      </c>
-      <c r="H1" t="str">
-        <v>5 năm</v>
-      </c>
-      <c r="I1" t="str">
-        <v>7 năm</v>
-      </c>
-      <c r="J1" t="str">
-        <v>10 năm</v>
-      </c>
-      <c r="K1" t="str">
-        <v>15 năm</v>
-      </c>
-      <c r="L1" t="str">
-        <v>20 năm</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>11-9-2023</v>
-      </c>
-      <c r="B2" t="str">
-        <v>1,7753078515566</v>
-      </c>
-      <c r="C2" t="str">
-        <v>1,79754174362707</v>
-      </c>
-      <c r="D2" t="str">
-        <v>1,81958072576587</v>
-      </c>
-      <c r="E2" t="str">
-        <v>1,84142524757549</v>
-      </c>
-      <c r="F2" t="str">
-        <v>1,92686773763566</v>
-      </c>
-      <c r="G2" t="str">
-        <v>2,00923495221759</v>
-      </c>
-      <c r="H2" t="str">
-        <v>2,16485970733411</v>
-      </c>
-      <c r="I2" t="str">
-        <v>2,30853294490001</v>
-      </c>
-      <c r="J2" t="str">
-        <v>2,50214821550541</v>
-      </c>
-      <c r="K2" t="str">
-        <v>2,76842971049249</v>
-      </c>
-      <c r="L2" t="str">
-        <v>2,9674263362508</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>10-9-2023</v>
-      </c>
-      <c r="B3" t="str">
-        <v>1,7753078515566</v>
-      </c>
-      <c r="C3" t="str">
-        <v>1,79754174362707</v>
-      </c>
-      <c r="D3" t="str">
-        <v>1,81958072576587</v>
-      </c>
-      <c r="E3" t="str">
-        <v>1,84142524757549</v>
-      </c>
-      <c r="F3" t="str">
-        <v>1,92686773763566</v>
-      </c>
-      <c r="G3" t="str">
-        <v>2,00923495221759</v>
-      </c>
-      <c r="H3" t="str">
-        <v>2,16485970733411</v>
-      </c>
-      <c r="I3" t="str">
-        <v>2,30853294490001</v>
-      </c>
-      <c r="J3" t="str">
-        <v>2,50214821550541</v>
-      </c>
-      <c r="K3" t="str">
-        <v>2,76842971049249</v>
-      </c>
-      <c r="L3" t="str">
-        <v>2,9674263362508</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
         <v>9-9-2023</v>
-      </c>
-      <c r="B4" t="str">
-        <v>1,7753078515566</v>
-      </c>
-      <c r="C4" t="str">
-        <v>1,79754174362707</v>
-      </c>
-      <c r="D4" t="str">
-        <v>1,81958072576587</v>
-      </c>
-      <c r="E4" t="str">
-        <v>1,84142524757549</v>
-      </c>
-      <c r="F4" t="str">
-        <v>1,92686773763566</v>
-      </c>
-      <c r="G4" t="str">
-        <v>2,00923495221759</v>
-      </c>
-      <c r="H4" t="str">
-        <v>2,16485970733411</v>
-      </c>
-      <c r="I4" t="str">
-        <v>2,30853294490001</v>
-      </c>
-      <c r="J4" t="str">
-        <v>2,50214821550541</v>
-      </c>
-      <c r="K4" t="str">
-        <v>2,76842971049249</v>
-      </c>
-      <c r="L4" t="str">
-        <v>2,9674263362508</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: crawl logic change
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,19 +397,1143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>3 tháng</v>
+      </c>
+      <c r="C1" t="str">
+        <v>6 tháng</v>
+      </c>
+      <c r="D1" t="str">
+        <v>9 tháng</v>
+      </c>
+      <c r="E1" t="str">
+        <v>1 năm</v>
+      </c>
+      <c r="F1" t="str">
+        <v>2 năm</v>
+      </c>
+      <c r="G1" t="str">
+        <v>3 năm</v>
+      </c>
+      <c r="H1" t="str">
+        <v>5 năm</v>
+      </c>
+      <c r="I1" t="str">
+        <v>7 năm</v>
+      </c>
+      <c r="J1" t="str">
+        <v>10 năm</v>
+      </c>
+      <c r="K1" t="str">
+        <v>15 năm</v>
+      </c>
+      <c r="L1" t="str">
+        <v>20 năm</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>1-8-2023</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2,05605323984699</v>
+      </c>
+      <c r="C2" t="str">
+        <v>2,05095768563259</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2,04723257416928</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2,0448125946974</v>
+      </c>
+      <c r="F2" t="str">
+        <v>2,04695695013901</v>
+      </c>
+      <c r="G2" t="str">
+        <v>2,06532770315437</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2,13842549950229</v>
+      </c>
+      <c r="I2" t="str">
+        <v>2,24353941309394</v>
+      </c>
+      <c r="J2" t="str">
+        <v>2,42936856552369</v>
+      </c>
+      <c r="K2" t="str">
+        <v>2,7393034244737</v>
+      </c>
+      <c r="L2" t="str">
+        <v>2,98860666369538</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2-8-2023</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1,90089183977571</v>
+      </c>
+      <c r="C3" t="str">
+        <v>1,91523128487472</v>
+      </c>
+      <c r="D3" t="str">
+        <v>1,92953729437542</v>
+      </c>
+      <c r="E3" t="str">
+        <v>1,94380989250891</v>
+      </c>
+      <c r="F3" t="str">
+        <v>2,0005666547757</v>
+      </c>
+      <c r="G3" t="str">
+        <v>2,05679077200289</v>
+      </c>
+      <c r="H3" t="str">
+        <v>2,16764729841001</v>
+      </c>
+      <c r="I3" t="str">
+        <v>2,27639197759153</v>
+      </c>
+      <c r="J3" t="str">
+        <v>2,43557683709068</v>
+      </c>
+      <c r="K3" t="str">
+        <v>2,69050509575799</v>
+      </c>
+      <c r="L3" t="str">
+        <v>2,93263246446584</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>3-8-2023</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1,78706730242217</v>
+      </c>
+      <c r="C4" t="str">
+        <v>1,79947180737767</v>
+      </c>
+      <c r="D4" t="str">
+        <v>1,81623207008519</v>
+      </c>
+      <c r="E4" t="str">
+        <v>1,83399464875147</v>
+      </c>
+      <c r="F4" t="str">
+        <v>1,90669417492002</v>
+      </c>
+      <c r="G4" t="str">
+        <v>1,97870370863449</v>
+      </c>
+      <c r="H4" t="str">
+        <v>2,1181009209166</v>
+      </c>
+      <c r="I4" t="str">
+        <v>2,25091043851786</v>
+      </c>
+      <c r="J4" t="str">
+        <v>2,43798142932199</v>
+      </c>
+      <c r="K4" t="str">
+        <v>2,71910861056437</v>
+      </c>
+      <c r="L4" t="str">
+        <v>2,96484499043859</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>4-8-2023</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1,7618043985917</v>
+      </c>
+      <c r="C5" t="str">
+        <v>1,76755378301832</v>
+      </c>
+      <c r="D5" t="str">
+        <v>1,78282486944494</v>
+      </c>
+      <c r="E5" t="str">
+        <v>1,80036554745246</v>
+      </c>
+      <c r="F5" t="str">
+        <v>1,87511027937417</v>
+      </c>
+      <c r="G5" t="str">
+        <v>1,94997298875144</v>
+      </c>
+      <c r="H5" t="str">
+        <v>2,0944518620329</v>
+      </c>
+      <c r="I5" t="str">
+        <v>2,23087941946034</v>
+      </c>
+      <c r="J5" t="str">
+        <v>2,42052223951859</v>
+      </c>
+      <c r="K5" t="str">
+        <v>2,69900836948513</v>
+      </c>
+      <c r="L5" t="str">
+        <v>2,9347713039797</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>5-8-2023</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>6-8-2023</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>7-8-2023</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1,87635176668532</v>
+      </c>
+      <c r="C8" t="str">
+        <v>1,89031813112714</v>
+      </c>
+      <c r="D8" t="str">
+        <v>1,90426142571352</v>
+      </c>
+      <c r="E8" t="str">
+        <v>1,91818168602167</v>
+      </c>
+      <c r="F8" t="str">
+        <v>1,97363309690741</v>
+      </c>
+      <c r="G8" t="str">
+        <v>2,02871880657072</v>
+      </c>
+      <c r="H8" t="str">
+        <v>2,13780220381605</v>
+      </c>
+      <c r="I8" t="str">
+        <v>2,24544998475962</v>
+      </c>
+      <c r="J8" t="str">
+        <v>2,40426925955182</v>
+      </c>
+      <c r="K8" t="str">
+        <v>2,66204385202737</v>
+      </c>
+      <c r="L8" t="str">
+        <v>2,91140263151293</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>8-8-2023</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1,8393986566112</v>
+      </c>
+      <c r="C9" t="str">
+        <v>1,85852178842547</v>
+      </c>
+      <c r="D9" t="str">
+        <v>1,87757043795533</v>
+      </c>
+      <c r="E9" t="str">
+        <v>1,89654467029632</v>
+      </c>
+      <c r="F9" t="str">
+        <v>1,97169873887471</v>
+      </c>
+      <c r="G9" t="str">
+        <v>2,04566739429906</v>
+      </c>
+      <c r="H9" t="str">
+        <v>2,19006548438232</v>
+      </c>
+      <c r="I9" t="str">
+        <v>2,32977331366497</v>
+      </c>
+      <c r="J9" t="str">
+        <v>2,53061729234132</v>
+      </c>
+      <c r="K9" t="str">
+        <v>2,8424073705694</v>
+      </c>
+      <c r="L9" t="str">
+        <v>3,12600516205508</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>9-8-2023</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1,85897378958828</v>
+      </c>
+      <c r="C10" t="str">
+        <v>1,87592282449525</v>
+      </c>
+      <c r="D10" t="str">
+        <v>1,8928467182979</v>
+      </c>
+      <c r="E10" t="str">
+        <v>1,90974545235671</v>
+      </c>
+      <c r="F10" t="str">
+        <v>1,97708909506173</v>
+      </c>
+      <c r="G10" t="str">
+        <v>2,04403130298416</v>
+      </c>
+      <c r="H10" t="str">
+        <v>2,17671464368443</v>
+      </c>
+      <c r="I10" t="str">
+        <v>2,30780203312813</v>
+      </c>
+      <c r="J10" t="str">
+        <v>2,50145529291019</v>
+      </c>
+      <c r="K10" t="str">
+        <v>2,81632656714681</v>
+      </c>
+      <c r="L10" t="str">
+        <v>3,12143707310881</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>10-8-2023</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1,91121046413081</v>
+      </c>
+      <c r="C11" t="str">
+        <v>1,92736051924289</v>
+      </c>
+      <c r="D11" t="str">
+        <v>1,94348534315867</v>
+      </c>
+      <c r="E11" t="str">
+        <v>1,95958495010051</v>
+      </c>
+      <c r="F11" t="str">
+        <v>2,02373153904778</v>
+      </c>
+      <c r="G11" t="str">
+        <v>2,08747594554983</v>
+      </c>
+      <c r="H11" t="str">
+        <v>2,213762187867</v>
+      </c>
+      <c r="I11" t="str">
+        <v>2,33845174367271</v>
+      </c>
+      <c r="J11" t="str">
+        <v>2,5225101433509</v>
+      </c>
+      <c r="K11" t="str">
+        <v>2,82140742695511</v>
+      </c>
+      <c r="L11" t="str">
+        <v>3,11058570972984</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>11-8-2023</v>
+      </c>
+      <c r="B12" t="str">
+        <v>1,86420721804454</v>
+      </c>
+      <c r="C12" t="str">
+        <v>1,88160290824055</v>
+      </c>
+      <c r="D12" t="str">
+        <v>1,89896593122534</v>
+      </c>
+      <c r="E12" t="str">
+        <v>1,9162962978764</v>
+      </c>
+      <c r="F12" t="str">
+        <v>1,98529142602697</v>
+      </c>
+      <c r="G12" t="str">
+        <v>2,05376495301195</v>
+      </c>
+      <c r="H12" t="str">
+        <v>2,18915012132421</v>
+      </c>
+      <c r="I12" t="str">
+        <v>2,32245772014958</v>
+      </c>
+      <c r="J12" t="str">
+        <v>2,51853693614783</v>
+      </c>
+      <c r="K12" t="str">
+        <v>2,83503522864219</v>
+      </c>
+      <c r="L12" t="str">
+        <v>3,13874575089361</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>12-8-2023</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>13-8-2023</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>14-8-2023</v>
+      </c>
+      <c r="B15" t="str">
+        <v>1,83812386032669</v>
+      </c>
+      <c r="C15" t="str">
+        <v>1,85567962709678</v>
+      </c>
+      <c r="D15" t="str">
+        <v>1,87320447614872</v>
+      </c>
+      <c r="E15" t="str">
+        <v>1,89069843205598</v>
+      </c>
+      <c r="F15" t="str">
+        <v>1,96036513934641</v>
+      </c>
+      <c r="G15" t="str">
+        <v>2,02953740540417</v>
+      </c>
+      <c r="H15" t="str">
+        <v>2,16639930376787</v>
+      </c>
+      <c r="I15" t="str">
+        <v>2,30128556292322</v>
+      </c>
+      <c r="J15" t="str">
+        <v>2,49991411771002</v>
+      </c>
+      <c r="K15" t="str">
+        <v>2,82110789895629</v>
+      </c>
+      <c r="L15" t="str">
+        <v>3,13001247474267</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>15-8-2023</v>
+      </c>
+      <c r="B16" t="str">
+        <v>1,83393934274212</v>
+      </c>
+      <c r="C16" t="str">
+        <v>1,85486822466576</v>
+      </c>
+      <c r="D16" t="str">
+        <v>1,87566550846023</v>
+      </c>
+      <c r="E16" t="str">
+        <v>1,89633181684101</v>
+      </c>
+      <c r="F16" t="str">
+        <v>1,97769972588449</v>
+      </c>
+      <c r="G16" t="str">
+        <v>2,05702164485675</v>
+      </c>
+      <c r="H16" t="str">
+        <v>2,20968513394684</v>
+      </c>
+      <c r="I16" t="str">
+        <v>2,3546352573439</v>
+      </c>
+      <c r="J16" t="str">
+        <v>2,55827323525875</v>
+      </c>
+      <c r="K16" t="str">
+        <v>2,86342693211346</v>
+      </c>
+      <c r="L16" t="str">
+        <v>3,12976989792248</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>16-8-2023</v>
+      </c>
+      <c r="B17" t="str">
+        <v>1,78557798144132</v>
+      </c>
+      <c r="C17" t="str">
+        <v>1,80924688087305</v>
+      </c>
+      <c r="D17" t="str">
+        <v>1,83266462317917</v>
+      </c>
+      <c r="E17" t="str">
+        <v>1,85583206698512</v>
+      </c>
+      <c r="F17" t="str">
+        <v>1,94601604004629</v>
+      </c>
+      <c r="G17" t="str">
+        <v>2,03226398894492</v>
+      </c>
+      <c r="H17" t="str">
+        <v>2,19317198851652</v>
+      </c>
+      <c r="I17" t="str">
+        <v>2,33899645374891</v>
+      </c>
+      <c r="J17" t="str">
+        <v>2,5304138149381</v>
+      </c>
+      <c r="K17" t="str">
+        <v>2,78024154272012</v>
+      </c>
+      <c r="L17" t="str">
+        <v>2,94944539051967</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>17-8-2023</v>
+      </c>
+      <c r="B18" t="str">
+        <v>1,82872827911889</v>
+      </c>
+      <c r="C18" t="str">
+        <v>1,93054262281458</v>
+      </c>
+      <c r="D18" t="str">
+        <v>2,00038400813158</v>
+      </c>
+      <c r="E18" t="str">
+        <v>2,04614373731726</v>
+      </c>
+      <c r="F18" t="str">
+        <v>2,09623293388281</v>
+      </c>
+      <c r="G18" t="str">
+        <v>2,07948049796709</v>
+      </c>
+      <c r="H18" t="str">
+        <v>2,11010984847413</v>
+      </c>
+      <c r="I18" t="str">
+        <v>2,24512300213084</v>
+      </c>
+      <c r="J18" t="str">
+        <v>2,49275289264539</v>
+      </c>
+      <c r="K18" t="str">
+        <v>2,80113720981758</v>
+      </c>
+      <c r="L18" t="str">
+        <v>2,98041551132962</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>18-8-2023</v>
+      </c>
+      <c r="B19" t="str">
+        <v>1,89448250283237</v>
+      </c>
+      <c r="C19" t="str">
+        <v>1,90762553197228</v>
+      </c>
+      <c r="D19" t="str">
+        <v>1,92075917915175</v>
+      </c>
+      <c r="E19" t="str">
+        <v>1,93388344748027</v>
+      </c>
+      <c r="F19" t="str">
+        <v>1,9862867941574</v>
+      </c>
+      <c r="G19" t="str">
+        <v>2,0385403270941</v>
+      </c>
+      <c r="H19" t="str">
+        <v>2,14259874787295</v>
+      </c>
+      <c r="I19" t="str">
+        <v>2,24606030716161</v>
+      </c>
+      <c r="J19" t="str">
+        <v>2,40013704467452</v>
+      </c>
+      <c r="K19" t="str">
+        <v>2,65397015341964</v>
+      </c>
+      <c r="L19" t="str">
+        <v>2,90412354612846</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>19-8-2023</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>20-8-2023</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>21-8-2023</v>
+      </c>
+      <c r="B22" t="str">
+        <v>1,86648499145341</v>
+      </c>
+      <c r="C22" t="str">
+        <v>1,8812839044706</v>
+      </c>
+      <c r="D22" t="str">
+        <v>1,89604552856026</v>
+      </c>
+      <c r="E22" t="str">
+        <v>1,91076988255021</v>
+      </c>
+      <c r="F22" t="str">
+        <v>1,96929508982235</v>
+      </c>
+      <c r="G22" t="str">
+        <v>2,02722593925406</v>
+      </c>
+      <c r="H22" t="str">
+        <v>2,14131085741003</v>
+      </c>
+      <c r="I22" t="str">
+        <v>2,25303730858342</v>
+      </c>
+      <c r="J22" t="str">
+        <v>2,41623290614017</v>
+      </c>
+      <c r="K22" t="str">
+        <v>2,67661646565165</v>
+      </c>
+      <c r="L22" t="str">
+        <v>2,92266793728668</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>22-8-2023</v>
+      </c>
+      <c r="B23" t="str">
+        <v>1,89584933168279</v>
+      </c>
+      <c r="C23" t="str">
+        <v>1,91241709612939</v>
+      </c>
+      <c r="D23" t="str">
+        <v>1,92889893295187</v>
+      </c>
+      <c r="E23" t="str">
+        <v>1,94529489878736</v>
+      </c>
+      <c r="F23" t="str">
+        <v>2,01002120127609</v>
+      </c>
+      <c r="G23" t="str">
+        <v>2,07337818203239</v>
+      </c>
+      <c r="H23" t="str">
+        <v>2,19599918647921</v>
+      </c>
+      <c r="I23" t="str">
+        <v>2,31318839811976</v>
+      </c>
+      <c r="J23" t="str">
+        <v>2,47885610031615</v>
+      </c>
+      <c r="K23" t="str">
+        <v>2,72826238377692</v>
+      </c>
+      <c r="L23" t="str">
+        <v>2,94474083368568</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>23-8-2023</v>
+      </c>
+      <c r="B24" t="str">
+        <v>1,78700625227488</v>
+      </c>
+      <c r="C24" t="str">
+        <v>1,80781854942209</v>
+      </c>
+      <c r="D24" t="str">
+        <v>1,8284714306456</v>
+      </c>
+      <c r="E24" t="str">
+        <v>1,84896502385576</v>
+      </c>
+      <c r="F24" t="str">
+        <v>1,92934909506495</v>
+      </c>
+      <c r="G24" t="str">
+        <v>2,0071949544721</v>
+      </c>
+      <c r="H24" t="str">
+        <v>2,15530623112123</v>
+      </c>
+      <c r="I24" t="str">
+        <v>2,29336896156409</v>
+      </c>
+      <c r="J24" t="str">
+        <v>2,48178199666529</v>
+      </c>
+      <c r="K24" t="str">
+        <v>2,74662889353221</v>
+      </c>
+      <c r="L24" t="str">
+        <v>2,95111042083085</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>24-8-2023</v>
+      </c>
+      <c r="B25" t="str">
+        <v>1,8074235952217</v>
+      </c>
+      <c r="C25" t="str">
+        <v>1,82583686672861</v>
+      </c>
+      <c r="D25" t="str">
+        <v>1,84434596601555</v>
+      </c>
+      <c r="E25" t="str">
+        <v>1,86293726250382</v>
+      </c>
+      <c r="F25" t="str">
+        <v>1,93786822413256</v>
+      </c>
+      <c r="G25" t="str">
+        <v>2,01314254424105</v>
+      </c>
+      <c r="H25" t="str">
+        <v>2,16215991637358</v>
+      </c>
+      <c r="I25" t="str">
+        <v>2,30575902953927</v>
+      </c>
+      <c r="J25" t="str">
+        <v>2,50468745985375</v>
+      </c>
+      <c r="K25" t="str">
+        <v>2,7791145773099</v>
+      </c>
+      <c r="L25" t="str">
+        <v>2,97531666752975</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>25-8-2023</v>
+      </c>
+      <c r="B26" t="str">
+        <v>1,79141512912448</v>
+      </c>
+      <c r="C26" t="str">
+        <v>1,811035087196</v>
+      </c>
+      <c r="D26" t="str">
+        <v>1,83053365220602</v>
+      </c>
+      <c r="E26" t="str">
+        <v>1,84991084376798</v>
+      </c>
+      <c r="F26" t="str">
+        <v>1,92620625732183</v>
+      </c>
+      <c r="G26" t="str">
+        <v>2,00056128797921</v>
+      </c>
+      <c r="H26" t="str">
+        <v>2,14345591181382</v>
+      </c>
+      <c r="I26" t="str">
+        <v>2,27860727546008</v>
+      </c>
+      <c r="J26" t="str">
+        <v>2,46684761956129</v>
+      </c>
+      <c r="K26" t="str">
+        <v>2,74209401652703</v>
+      </c>
+      <c r="L26" t="str">
+        <v>2,9695084370829</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>26-8-2023</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>27-8-2023</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>28-8-2023</v>
+      </c>
+      <c r="B29" t="str">
+        <v>1,75881544453373</v>
+      </c>
+      <c r="C29" t="str">
+        <v>1,8040813632221</v>
+      </c>
+      <c r="D29" t="str">
+        <v>1,84201863444673</v>
+      </c>
+      <c r="E29" t="str">
+        <v>1,87398274720791</v>
+      </c>
+      <c r="F29" t="str">
+        <v>1,96264417279566</v>
+      </c>
+      <c r="G29" t="str">
+        <v>2,02119943608083</v>
+      </c>
+      <c r="H29" t="str">
+        <v>2,12988820800168</v>
+      </c>
+      <c r="I29" t="str">
+        <v>2,26021211324623</v>
+      </c>
+      <c r="J29" t="str">
+        <v>2,47611578975651</v>
+      </c>
+      <c r="K29" t="str">
+        <v>2,78904196774579</v>
+      </c>
+      <c r="L29" t="str">
+        <v>3,0044657334007</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>29-8-2023</v>
+      </c>
+      <c r="B30" t="str">
+        <v>1,78638624345486</v>
+      </c>
+      <c r="C30" t="str">
+        <v>1,81003875188701</v>
+      </c>
+      <c r="D30" t="str">
+        <v>1,83346249062397</v>
+      </c>
+      <c r="E30" t="str">
+        <v>1,85665831614308</v>
+      </c>
+      <c r="F30" t="str">
+        <v>1,94717958242086</v>
+      </c>
+      <c r="G30" t="str">
+        <v>2,03412251198969</v>
+      </c>
+      <c r="H30" t="str">
+        <v>2,19749053617602</v>
+      </c>
+      <c r="I30" t="str">
+        <v>2,34719405219079</v>
+      </c>
+      <c r="J30" t="str">
+        <v>2,54706123482631</v>
+      </c>
+      <c r="K30" t="str">
+        <v>2,81782749489921</v>
+      </c>
+      <c r="L30" t="str">
+        <v>3,01618634379648</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>30-8-2023</v>
+      </c>
+      <c r="B31" t="str">
+        <v>1,80043886360692</v>
+      </c>
+      <c r="C31" t="str">
+        <v>1,80923755279661</v>
+      </c>
+      <c r="D31" t="str">
+        <v>1,81963718577993</v>
+      </c>
+      <c r="E31" t="str">
+        <v>1,83150949587945</v>
+      </c>
+      <c r="F31" t="str">
+        <v>1,89139740758844</v>
+      </c>
+      <c r="G31" t="str">
+        <v>1,96626630794081</v>
+      </c>
+      <c r="H31" t="str">
+        <v>2,14061088045627</v>
+      </c>
+      <c r="I31" t="str">
+        <v>2,32414931061924</v>
+      </c>
+      <c r="J31" t="str">
+        <v>2,57994500024603</v>
+      </c>
+      <c r="K31" t="str">
+        <v>2,8999476910164</v>
+      </c>
+      <c r="L31" t="str">
+        <v>3,08184483685607</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>31-8-2023</v>
+      </c>
+      <c r="B32" t="str">
+        <v>1,82878052894908</v>
+      </c>
+      <c r="C32" t="str">
+        <v>1,85033117100568</v>
+      </c>
+      <c r="D32" t="str">
+        <v>1,87168778741345</v>
+      </c>
+      <c r="E32" t="str">
+        <v>1,89284981831113</v>
+      </c>
+      <c r="F32" t="str">
+        <v>1,97557366673677</v>
+      </c>
+      <c r="G32" t="str">
+        <v>2,05527902297022</v>
+      </c>
+      <c r="H32" t="str">
+        <v>2,20595677684725</v>
+      </c>
+      <c r="I32" t="str">
+        <v>2,34551205065905</v>
+      </c>
+      <c r="J32" t="str">
+        <v>2,53529795610787</v>
+      </c>
+      <c r="K32" t="str">
+        <v>2,8041257365347</v>
+      </c>
+      <c r="L32" t="str">
+        <v>3,02049886264641</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>1-9-2023</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>2-9-2023</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>3-9-2023</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>4-9-2023</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>5-9-2023</v>
+      </c>
+      <c r="B37" t="str">
+        <v>1,90602171119172</v>
+      </c>
+      <c r="C37" t="str">
+        <v>1,91237046272037</v>
+      </c>
+      <c r="D37" t="str">
+        <v>1,91994319250539</v>
+      </c>
+      <c r="E37" t="str">
+        <v>1,92864565831672</v>
+      </c>
+      <c r="F37" t="str">
+        <v>1,97304658727595</v>
+      </c>
+      <c r="G37" t="str">
+        <v>2,02924528729085</v>
+      </c>
+      <c r="H37" t="str">
+        <v>2,16224978499429</v>
+      </c>
+      <c r="I37" t="str">
+        <v>2,30563479064041</v>
+      </c>
+      <c r="J37" t="str">
+        <v>2,51352414098844</v>
+      </c>
+      <c r="K37" t="str">
+        <v>2,79985635260103</v>
+      </c>
+      <c r="L37" t="str">
+        <v>3,00176431311514</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>6-9-2023</v>
+      </c>
+      <c r="B38" t="str">
+        <v>1,80390472256851</v>
+      </c>
+      <c r="C38" t="str">
+        <v>1,82553117790643</v>
+      </c>
+      <c r="D38" t="str">
+        <v>1,84721202352272</v>
+      </c>
+      <c r="E38" t="str">
+        <v>1,86893001751289</v>
+      </c>
+      <c r="F38" t="str">
+        <v>1,95585301673042</v>
+      </c>
+      <c r="G38" t="str">
+        <v>2,04216659469669</v>
+      </c>
+      <c r="H38" t="str">
+        <v>2,20991236219314</v>
+      </c>
+      <c r="I38" t="str">
+        <v>2,3673318939587</v>
+      </c>
+      <c r="J38" t="str">
+        <v>2,57760214859364</v>
+      </c>
+      <c r="K38" t="str">
+        <v>2,8485861380201</v>
+      </c>
+      <c r="L38" t="str">
+        <v>3,02088147025283</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>7-9-2023</v>
+      </c>
+      <c r="B39" t="str">
+        <v>1,77113805484441</v>
+      </c>
+      <c r="C39" t="str">
+        <v>1,79465409429311</v>
+      </c>
+      <c r="D39" t="str">
+        <v>1,81799070932709</v>
+      </c>
+      <c r="E39" t="str">
+        <v>1,8411479319544</v>
+      </c>
+      <c r="F39" t="str">
+        <v>1,93198361191003</v>
+      </c>
+      <c r="G39" t="str">
+        <v>2,01995196976916</v>
+      </c>
+      <c r="H39" t="str">
+        <v>2,18729746462321</v>
+      </c>
+      <c r="I39" t="str">
+        <v>2,34320839636104</v>
+      </c>
+      <c r="J39" t="str">
+        <v>2,55569712154196</v>
+      </c>
+      <c r="K39" t="str">
+        <v>2,85312263097162</v>
+      </c>
+      <c r="L39" t="str">
+        <v>3,0802027523277</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>8-9-2023</v>
+      </c>
+      <c r="B40" t="str">
+        <v>1,79265122504342</v>
+      </c>
+      <c r="C40" t="str">
+        <v>1,81220032531189</v>
+      </c>
+      <c r="D40" t="str">
+        <v>1,83164280401553</v>
+      </c>
+      <c r="E40" t="str">
+        <v>1,85097865893171</v>
+      </c>
+      <c r="F40" t="str">
+        <v>1,9272554985408</v>
+      </c>
+      <c r="G40" t="str">
+        <v>2,0018251696819</v>
+      </c>
+      <c r="H40" t="str">
+        <v>2,14583994905106</v>
+      </c>
+      <c r="I40" t="str">
+        <v>2,28301778448015</v>
+      </c>
+      <c r="J40" t="str">
+        <v>2,47595742190916</v>
+      </c>
+      <c r="K40" t="str">
+        <v>2,76330587879252</v>
+      </c>
+      <c r="L40" t="str">
+        <v>3,00789896772866</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
         <v>9-9-2023</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L41"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>